<commit_message>
small silkscreen touchup and regenerated gerbers
</commit_message>
<xml_diff>
--- a/bitaxe BOM.xlsx
+++ b/bitaxe BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{343B862D-2819-3A47-B624-52FBA774E778}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{172A0FF0-4D9B-5D4B-80C7-618F710B4E95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15740" yWindow="6020" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="15720" yWindow="6020" windowWidth="28040" windowHeight="17440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxe" sheetId="1" r:id="rId1"/>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>